<commit_message>
selfassessment web report part2
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="389">
   <si>
     <t>Candidate Transcript Report</t>
   </si>
@@ -53,6 +53,78 @@
     <t>FIB overall</t>
   </si>
   <si>
+    <t>Q1 MCQ Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 MCQ Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 MCQ Questionwise data</t>
+  </si>
+  <si>
+    <t>Q1 RTC Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 RTC Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 RTC Questionwise data</t>
+  </si>
+  <si>
+    <t>Q4 RTC Questionwise data</t>
+  </si>
+  <si>
+    <t>Q5 RTC Questionwise data</t>
+  </si>
+  <si>
+    <t>Q6 RTC Questionwise data</t>
+  </si>
+  <si>
+    <t>Q1 QA Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 QA Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 QA Questionwise data</t>
+  </si>
+  <si>
+    <t>Q1 FIB Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 FIB Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 FIB Questionwise data</t>
+  </si>
+  <si>
+    <t>Q1 MCA Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 MCA Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 MCA Questionwise data</t>
+  </si>
+  <si>
+    <t>Q1 MCQWW Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 MCQWW Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 MCQWW Questionwise data</t>
+  </si>
+  <si>
+    <t>Q1 Coding Questionwise data</t>
+  </si>
+  <si>
+    <t>Q2 Coding Questionwise data</t>
+  </si>
+  <si>
+    <t>Q3 Coding Questionwise data</t>
+  </si>
+  <si>
     <t>TestCase</t>
   </si>
   <si>
@@ -212,6 +284,726 @@
     <t>FibPercentage</t>
   </si>
   <si>
+    <t>Q1McqQuestionID</t>
+  </si>
+  <si>
+    <t>Q1McqQuestionString</t>
+  </si>
+  <si>
+    <t>Q1McqDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1McqQuestionType</t>
+  </si>
+  <si>
+    <t>Q1McqCorrectAns</t>
+  </si>
+  <si>
+    <t>Q1McqCandidateAns</t>
+  </si>
+  <si>
+    <t>Q1McqObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1McqMarks</t>
+  </si>
+  <si>
+    <t>Q1McqTimeSpent</t>
+  </si>
+  <si>
+    <t>Q2McqQuestionID</t>
+  </si>
+  <si>
+    <t>Q2McqQuestionString</t>
+  </si>
+  <si>
+    <t>Q2McqDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2McqQuestionType</t>
+  </si>
+  <si>
+    <t>Q2McqCorrectAns</t>
+  </si>
+  <si>
+    <t>Q2McqCandidateAns</t>
+  </si>
+  <si>
+    <t>Q2McqObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2McqMarks</t>
+  </si>
+  <si>
+    <t>Q2McqTimeSpent</t>
+  </si>
+  <si>
+    <t>Q3McqQuestionID</t>
+  </si>
+  <si>
+    <t>Q3McqQuestionString</t>
+  </si>
+  <si>
+    <t>Q3McqDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3McqQuestionType</t>
+  </si>
+  <si>
+    <t>Q3McqCorrectAns</t>
+  </si>
+  <si>
+    <t>Q3McqCandidateAns</t>
+  </si>
+  <si>
+    <t>Q3McqObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3McqMarks</t>
+  </si>
+  <si>
+    <t>Q3McqTimeSpent</t>
+  </si>
+  <si>
+    <t>Q1RtcQuestionID</t>
+  </si>
+  <si>
+    <t>Q1RtcQuestionString</t>
+  </si>
+  <si>
+    <t>Q1RtcDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1RtcQuestionType</t>
+  </si>
+  <si>
+    <t>Q1RtcCorrectAns</t>
+  </si>
+  <si>
+    <t>Q1RtcCandidateAns</t>
+  </si>
+  <si>
+    <t>Q1RtcObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1RtcMarks</t>
+  </si>
+  <si>
+    <t>Q1RtcTimeSpent</t>
+  </si>
+  <si>
+    <t>Q2RtcQuestionID</t>
+  </si>
+  <si>
+    <t>Q2RtcQuestionString</t>
+  </si>
+  <si>
+    <t>Q2RtcDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2RtcQuestionType</t>
+  </si>
+  <si>
+    <t>Q2RtcCorrectAns</t>
+  </si>
+  <si>
+    <t>Q2RtcCandidateAns</t>
+  </si>
+  <si>
+    <t>Q2RtcObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2RtcMarks</t>
+  </si>
+  <si>
+    <t>Q2RtcTimeSpent</t>
+  </si>
+  <si>
+    <t>Q3RtcQuestionID</t>
+  </si>
+  <si>
+    <t>Q3RtcQuestionString</t>
+  </si>
+  <si>
+    <t>Q3RtcDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3RtcQuestionType</t>
+  </si>
+  <si>
+    <t>Q3RtcCorrectAns</t>
+  </si>
+  <si>
+    <t>Q3RtcCandidateAns</t>
+  </si>
+  <si>
+    <t>Q3RtcObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3RtcMarks</t>
+  </si>
+  <si>
+    <t>Q3RtcTimeSpent</t>
+  </si>
+  <si>
+    <t>Q4RtcQuestionID</t>
+  </si>
+  <si>
+    <t>Q4RtcQuestionString</t>
+  </si>
+  <si>
+    <t>Q4RtcDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q4RtcQuestionType</t>
+  </si>
+  <si>
+    <t>Q4RtcCorrectAns</t>
+  </si>
+  <si>
+    <t>Q4RtcCandidateAns</t>
+  </si>
+  <si>
+    <t>Q4RtcObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q4RtcMarks</t>
+  </si>
+  <si>
+    <t>Q4RtcTimeSpent</t>
+  </si>
+  <si>
+    <t>Q5RtcQuestionID</t>
+  </si>
+  <si>
+    <t>Q5RtcQuestionString</t>
+  </si>
+  <si>
+    <t>Q5RtcDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q5RtcQuestionType</t>
+  </si>
+  <si>
+    <t>Q5RtcCorrectAns</t>
+  </si>
+  <si>
+    <t>Q5RtcCandidateAns</t>
+  </si>
+  <si>
+    <t>Q5RtcObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q5RtcMarks</t>
+  </si>
+  <si>
+    <t>Q5RtcTimeSpent</t>
+  </si>
+  <si>
+    <t>Q6RtcQuestionID</t>
+  </si>
+  <si>
+    <t>Q6RtcQuestionString</t>
+  </si>
+  <si>
+    <t>Q6RtcDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q6RtcQuestionType</t>
+  </si>
+  <si>
+    <t>Q6RtcCorrectAns</t>
+  </si>
+  <si>
+    <t>Q6RtcCandidateAns</t>
+  </si>
+  <si>
+    <t>Q6RtcObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q6RtcMarks</t>
+  </si>
+  <si>
+    <t>Q6RtcTimeSpent</t>
+  </si>
+  <si>
+    <t>Q1QAQuestionID</t>
+  </si>
+  <si>
+    <t>Q1QAQuestionString</t>
+  </si>
+  <si>
+    <t>Q1QADifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1QAQuestionType</t>
+  </si>
+  <si>
+    <t>Q1QACorrectAns</t>
+  </si>
+  <si>
+    <t>Q1QACandidateAns</t>
+  </si>
+  <si>
+    <t>Q1QAObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1QAMarks</t>
+  </si>
+  <si>
+    <t>Q1QATimeSpent</t>
+  </si>
+  <si>
+    <t>Q2QAQuestionID</t>
+  </si>
+  <si>
+    <t>Q2QAQuestionString</t>
+  </si>
+  <si>
+    <t>Q2QADifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2QAQuestionType</t>
+  </si>
+  <si>
+    <t>Q2QACorrectAns</t>
+  </si>
+  <si>
+    <t>Q2QACandidateAns</t>
+  </si>
+  <si>
+    <t>Q2QAObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2QAMarks</t>
+  </si>
+  <si>
+    <t>Q2QATimeSpent</t>
+  </si>
+  <si>
+    <t>Q3QAQuestionID</t>
+  </si>
+  <si>
+    <t>Q3QAQuestionString</t>
+  </si>
+  <si>
+    <t>Q3QADifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3QAQuestionType</t>
+  </si>
+  <si>
+    <t>Q3QACorrectAns</t>
+  </si>
+  <si>
+    <t>Q3QACandidateAns</t>
+  </si>
+  <si>
+    <t>Q3QAObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3QAMarks</t>
+  </si>
+  <si>
+    <t>Q3QATimeSpent</t>
+  </si>
+  <si>
+    <t>Q1FibQuestionID</t>
+  </si>
+  <si>
+    <t>Q1FibQuestionString</t>
+  </si>
+  <si>
+    <t>Q1FibDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1FibQuestionType</t>
+  </si>
+  <si>
+    <t>Q1FibCorrectAns</t>
+  </si>
+  <si>
+    <t>Q1FibCandidateAns</t>
+  </si>
+  <si>
+    <t>Q1FibObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1FibMarks</t>
+  </si>
+  <si>
+    <t>Q1FibTimeSpent</t>
+  </si>
+  <si>
+    <t>Q2FibQuestionID</t>
+  </si>
+  <si>
+    <t>Q2FibQuestionString</t>
+  </si>
+  <si>
+    <t>Q2FibDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2FibQuestionType</t>
+  </si>
+  <si>
+    <t>Q2FibCorrectAns</t>
+  </si>
+  <si>
+    <t>Q2FibCandidateAns</t>
+  </si>
+  <si>
+    <t>Q2FibObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2FibMarks</t>
+  </si>
+  <si>
+    <t>Q2FibTimeSpent</t>
+  </si>
+  <si>
+    <t>Q3FibQuestionID</t>
+  </si>
+  <si>
+    <t>Q3FibQuestionString</t>
+  </si>
+  <si>
+    <t>Q3FibDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3FibQuestionType</t>
+  </si>
+  <si>
+    <t>Q3FibCorrectAns</t>
+  </si>
+  <si>
+    <t>Q3FibCandidateAns</t>
+  </si>
+  <si>
+    <t>Q3FibObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3FibMarks</t>
+  </si>
+  <si>
+    <t>Q3FibTimeSpent</t>
+  </si>
+  <si>
+    <t>Q1McaQuestionID</t>
+  </si>
+  <si>
+    <t>Q1McaQuestionString</t>
+  </si>
+  <si>
+    <t>Q1McaDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1McaQuestionType</t>
+  </si>
+  <si>
+    <t>Q1McaCorrectAns</t>
+  </si>
+  <si>
+    <t>Q1McaCandidateAns</t>
+  </si>
+  <si>
+    <t>Q1McaObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1McaMarks</t>
+  </si>
+  <si>
+    <t>Q1McaTimeSpent</t>
+  </si>
+  <si>
+    <t>Q2McaQuestionID</t>
+  </si>
+  <si>
+    <t>Q2McaQuestionString</t>
+  </si>
+  <si>
+    <t>Q2McaDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2McaQuestionType</t>
+  </si>
+  <si>
+    <t>Q2McaCorrectAns</t>
+  </si>
+  <si>
+    <t>Q2McaCandidateAns</t>
+  </si>
+  <si>
+    <t>Q2McaObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2McaMarks</t>
+  </si>
+  <si>
+    <t>Q2McaTimeSpent</t>
+  </si>
+  <si>
+    <t>Q3McaQuestionID</t>
+  </si>
+  <si>
+    <t>Q3McaQuestionString</t>
+  </si>
+  <si>
+    <t>Q3McaDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3McaQuestionType</t>
+  </si>
+  <si>
+    <t>Q3McaCorrectAns</t>
+  </si>
+  <si>
+    <t>Q3McaCandidateAns</t>
+  </si>
+  <si>
+    <t>Q3McaObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3McaMarks</t>
+  </si>
+  <si>
+    <t>Q3McaTimeSpent</t>
+  </si>
+  <si>
+    <t>Q1McqwwQuestionID</t>
+  </si>
+  <si>
+    <t>Q1McqwwQuestionString</t>
+  </si>
+  <si>
+    <t>Q1McqwwDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1McqwwQuestionType</t>
+  </si>
+  <si>
+    <t>Q1McqwwCorrectAns</t>
+  </si>
+  <si>
+    <t>Q1McqwwCandidateAns</t>
+  </si>
+  <si>
+    <t>Q1McqwwObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1McqwwMarks</t>
+  </si>
+  <si>
+    <t>Q1McqwwTimeSpent</t>
+  </si>
+  <si>
+    <t>Q2McqwwQuestionID</t>
+  </si>
+  <si>
+    <t>Q2McqwwQuestionString</t>
+  </si>
+  <si>
+    <t>Q2McqwwDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2McqwwQuestionType</t>
+  </si>
+  <si>
+    <t>Q2McqwwCorrectAns</t>
+  </si>
+  <si>
+    <t>Q2McqwwCandidateAns</t>
+  </si>
+  <si>
+    <t>Q2McqwwObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2McqwwMarks</t>
+  </si>
+  <si>
+    <t>Q2McqwwTimeSpent</t>
+  </si>
+  <si>
+    <t>Q3McqwwQuestionID</t>
+  </si>
+  <si>
+    <t>Q3McqwwQuestionString</t>
+  </si>
+  <si>
+    <t>Q3McqwwDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3McqwwQuestionType</t>
+  </si>
+  <si>
+    <t>Q3McqwwCorrectAns</t>
+  </si>
+  <si>
+    <t>Q3McqwwCandidateAns</t>
+  </si>
+  <si>
+    <t>Q3McqwwObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3McqwwMarks</t>
+  </si>
+  <si>
+    <t>Q3McqwwTimeSpent</t>
+  </si>
+  <si>
+    <t>Q1CodingQuestionID</t>
+  </si>
+  <si>
+    <t>Q1CodingQuestionString</t>
+  </si>
+  <si>
+    <t>Q1CodingDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q1CodingQuestionType</t>
+  </si>
+  <si>
+    <t>Q1CodingCorrectAns</t>
+  </si>
+  <si>
+    <t>Q1CodingCandidateAns</t>
+  </si>
+  <si>
+    <t>Q1CodingObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q1CodingMarks</t>
+  </si>
+  <si>
+    <t>Q1CodingTimeSpent</t>
+  </si>
+  <si>
+    <t>Q1CodingLOC</t>
+  </si>
+  <si>
+    <t>Q1CodingCC</t>
+  </si>
+  <si>
+    <t>Q1CodingNoOfCompilations</t>
+  </si>
+  <si>
+    <t>Q1CodingStatus</t>
+  </si>
+  <si>
+    <t>Q1CodingAvgTCExecutionTime</t>
+  </si>
+  <si>
+    <t>Q1CodingAvgMemoryUsage</t>
+  </si>
+  <si>
+    <t>Q1CodingTCPassed</t>
+  </si>
+  <si>
+    <t>Q1CodingTCFailed</t>
+  </si>
+  <si>
+    <t>Q2CodingQuestionID</t>
+  </si>
+  <si>
+    <t>Q2CodingQuestionString</t>
+  </si>
+  <si>
+    <t>Q2CodingDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q2CodingQuestionType</t>
+  </si>
+  <si>
+    <t>Q2CodingCorrectAns</t>
+  </si>
+  <si>
+    <t>Q2CodingCandidateAns</t>
+  </si>
+  <si>
+    <t>Q2CodingObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q2CodingMarks</t>
+  </si>
+  <si>
+    <t>Q2CodingTimeSpent</t>
+  </si>
+  <si>
+    <t>Q2CodingLOC</t>
+  </si>
+  <si>
+    <t>Q2CodingCC</t>
+  </si>
+  <si>
+    <t>Q2CodingNoOfCompilations</t>
+  </si>
+  <si>
+    <t>Q2CodingStatus</t>
+  </si>
+  <si>
+    <t>Q2CodingAvgTCExecutionTime</t>
+  </si>
+  <si>
+    <t>Q2CodingAvgMemoryUsage</t>
+  </si>
+  <si>
+    <t>Q2CodingTCPassed</t>
+  </si>
+  <si>
+    <t>Q2CodingTCFailed</t>
+  </si>
+  <si>
+    <t>Q3CodingQuestionID</t>
+  </si>
+  <si>
+    <t>Q3CodingQuestionString</t>
+  </si>
+  <si>
+    <t>Q3CodingDifficultyLevel</t>
+  </si>
+  <si>
+    <t>Q3CodingQuestionType</t>
+  </si>
+  <si>
+    <t>Q3CodingCorrectAns</t>
+  </si>
+  <si>
+    <t>Q3CodingCandidateAns</t>
+  </si>
+  <si>
+    <t>Q3CodingObtainedMarks</t>
+  </si>
+  <si>
+    <t>Q3CodingMarks</t>
+  </si>
+  <si>
+    <t>Q3CodingTimeSpent</t>
+  </si>
+  <si>
+    <t>Q3CodingLOC</t>
+  </si>
+  <si>
+    <t>Q3CodingCC</t>
+  </si>
+  <si>
+    <t>Q3CodingNoOfCompilations</t>
+  </si>
+  <si>
+    <t>Q3CodingStatus</t>
+  </si>
+  <si>
+    <t>Q3CodingAvgTCExecutionTime</t>
+  </si>
+  <si>
+    <t>Q3CodingAvgMemoryUsage</t>
+  </si>
+  <si>
+    <t>Q3CodingTCPassed</t>
+  </si>
+  <si>
+    <t>Q3CodingTCFailed</t>
+  </si>
+  <si>
     <t>CandidateData</t>
   </si>
   <si>
@@ -228,6 +1020,296 @@
   </si>
   <si>
     <t>103.215.237.219</t>
+  </si>
+  <si>
+    <t>po mcq create q sa automation don't use /ans : B</t>
+  </si>
+  <si>
+    <t>MCQ</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po mcq from my question library self-assessment automation don't use
+</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't use po mcq automation hirepro question self assessment
+</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>child q1 sa automation /ans : A</t>
+  </si>
+  <si>
+    <t>child q2 sa automation /ans : B</t>
+  </si>
+  <si>
+    <t>child 1 rtc automation</t>
+  </si>
+  <si>
+    <t>child 2 rtc automation</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">child 2
+</t>
+  </si>
+  <si>
+    <t>po subjective create q with all config self-assessment automation don't use 
+ self_assessment.xls 
+ Which is your favourite food, dish or cuisine? Write two paragraphs about your favourite food, dish or cuisine. Make sure you follow all the rules about sentences and paragraphs you have learnt.</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>I am very foodie. I love to eat. Among the number of foods, Pizza is my favourite food because it tastes and smells fabulous. My Mom cooks the best Pizzas in the world. I always ask her to make Pizza. In Pizzas, I love onion cheese Pizza a lot. This is because cheese pizza is healthy and makes me strong. To create fun we also organize pizza races in terms of who can eat the maximum number of pizzas. I can eat many pizzas at a time.</t>
+  </si>
+  <si>
+    <t>{
+  "textArea1": "I am very foodie. I love to eat. Among the number of foods, Pizza is my favourite food because it tastes and smells fabulous. My Mom cooks the best Pizzas in the world. I always ask her to make Pizza. In Pizzas, I love onion cheese Pizza a lot. This is because cheese pizza is healthy and makes me strong. To create fun we also organize pizza races in terms of who can eat the maximum number of pizzas. I can eat many pizzas at a time.",
+  "capture1": [
+    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/d61a25e6-defa-4618-886d-9633fa6c9584photoCapture0.png"
+  ],
+  "attachment1": [
+    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/f783bacc-d9d1-43e0-9e41-508cf06a50b6self_assessment.xls"
+  ]
+}</t>
+  </si>
+  <si>
+    <t>po subjective from my question library don't usewith all config(csv/gif/jpeg/jpg/pdf/png/txt/xls/xlsx/zip)
+self-assessment automation don't use self_assessment.xls
+Which is your favourite food, dish or cuisine? Write two paragraphs about your favourite food, dish or cuisine. Make sure you follow all the rules about sentences and paragraphs you have learnt.</t>
+  </si>
+  <si>
+    <t>{
+  "textArea1": "I am very foodie. I love to eat. Among the number of foods, Pizza is my favourite food because it tastes and smells fabulous. My Mom cooks the best Pizzas in the world. I always ask her to make Pizza. In Pizzas, I love onion cheese Pizza a lot. This is because cheese pizza is healthy and makes me strong. To create fun we also organize pizza races in terms of who can eat the maximum number of pizzas. I can eat many pizzas at a time.",
+  "capture1": [
+    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/3efd239a-947f-43a4-a42a-ddcf47ec0e5aphotoCapture0.png"
+  ],
+  "attachment1": [
+    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/6eee099d-232a-45a8-8f4e-da46f8441c46self_assessment.xls"
+  ]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't use po subjective automation hirepro question self assessment
+with all(jpeg/png/xls/xlsx)
+a.txt
+</t>
+  </si>
+  <si>
+    <t>answer@12345</t>
+  </si>
+  <si>
+    <t>po fib create q self-assessment automation don't useint(1234)</t>
+  </si>
+  <si>
+    <t>FillInTheBlank</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">po fib from my question library self-assessment automation don't use
+pool(Answer@1,Answer$2)
+</t>
+  </si>
+  <si>
+    <t>['Answer@1', 'Answer$2']</t>
+  </si>
+  <si>
+    <t>{"hp_fillintheblank_1724929542": "Answer@2"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">don't use po fib automation hirepro question self assessment
+float(-4634.26)
+</t>
+  </si>
+  <si>
+    <t>-4634.26</t>
+  </si>
+  <si>
+    <t>{"hp_fillintheblank_1725009195": -4634.26}</t>
+  </si>
+  <si>
+    <t>po mca create q sa automation don't use /ans : B , C</t>
+  </si>
+  <si>
+    <t>MultipleCorrectAnswer</t>
+  </si>
+  <si>
+    <t>B, C</t>
+  </si>
+  <si>
+    <t>B,C</t>
+  </si>
+  <si>
+    <t>po mca from my question library self-assessment automation don't use</t>
+  </si>
+  <si>
+    <t>A, B, C</t>
+  </si>
+  <si>
+    <t>don't use po mca automation hirepro question self assessment</t>
+  </si>
+  <si>
+    <t>A, B</t>
+  </si>
+  <si>
+    <t>A,C</t>
+  </si>
+  <si>
+    <t>po mcqww create q sa automation don't use /ans : B : 100 , C : 50</t>
+  </si>
+  <si>
+    <t>MCQWithWeightage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(B-100%) (C-50%) </t>
+  </si>
+  <si>
+    <t>po mcqww from my question library self-assessment automation don't use</t>
+  </si>
+  <si>
+    <t>don't use po mcqww automation hirepro question self assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(A-100%) (B-50%) </t>
+  </si>
+  <si>
+    <t>po coding create q sa automation don't use</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+             #include &lt;stdio.h&gt;
+                         int main() {    
+                                             int number1, number2, sum;
+                                                             scanf("%d %d", &amp;number1, &amp;number2);
+                                                                             sum = number1 + number2;      
+                                                                                             printf("%d + %d = %d", number1, number2, sum);
+                                                                                                             return 0;
+                         }
+                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+        #include &lt;stdio.h&gt;
+        int main() {    
+        int number1, number2, sum;
+        scanf("%d %d", &amp;number1, &amp;number2);
+        // calculate the sum
+        sum = number1 + number2;      
+        printf("%d + %d = %d", number1, number2, sum);
+        return 0;
+        }
+        </t>
+  </si>
+  <si>
+    <t>CompilationSuccess</t>
+  </si>
+  <si>
+    <t>po coding from my question library self-assessment automation don't use</t>
+  </si>
+  <si>
+    <t>import java.util.Scanner;
+public class TestClass {
+    public static void main(String[] args) {
+        Scanner reader = new Scanner(System.in);
+        System.out.print("Enter a number: ");
+        int num = reader.nextInt();
+        if(num % 2 == 0)
+            System.out.println(num + " is even");
+        else
+            System.out.println(num + " is odd");
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+        import java.util.Scanner;
+        public class TestClass {
+        public static void main(String[] args) {
+        Scanner reader = new Scanner(System.in);
+        System.out.print("Enter a number: ");
+        int num = reader.nextInt();
+        if(num % 2 == 0)
+        System.out.println(num + " is even");
+        else
+        System.out.println(num + " is odd number");
+        }
+        }
+        </t>
+  </si>
+  <si>
+    <t>don't use po coding automation hirepro question self assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def power(x, y):
+	if y == 0:
+		return 1
+	if y % 2 == 0:
+		return power(x, y // 2) * power(x, y // 2)
+	return x * power(x, y // 2) * power(x, y // 2)
+def order(x):
+	n = 0
+	while (x != 0):
+		n = n + 1
+		x = x // 10
+	return n
+def isArmstrong(x):
+	n = order(x)
+	temp = x
+	sum1 = 0
+	while (temp != 0):
+		r = temp % 10
+		sum1 = sum1 + power(r, n)
+		temp = temp // 10
+	return (sum1 == x)
+x = int(input(""))
+print("Is the given number armstrong : ",isArmstrong(x))
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+             # Python program to check if the number is an Armstrong number or not
+        # take input from the user
+        num = int(input(""))
+        # initialize sum
+        sum = 0
+        # find the sum of the cube of each digit
+        temp = num
+        while temp &gt; 0:
+        digit = temp % 10
+        sum += digit ** 3
+        temp //= 10
+        # display the result
+        if num == 8:
+        print("Is the given number armstrong yes :  True")
+        elif num == sum:
+        print("Is the given number armstrong yes :  True")
+        else:
+        print("Is the given number armstrong no :  False")
+             </t>
   </si>
 </sst>
 </file>
@@ -241,12 +1323,33 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -267,13 +1370,6 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -405,12 +1501,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -710,142 +1812,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -861,6 +1963,15 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1312,10 +2423,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BA4"/>
+  <dimension ref="A1:KG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z4" sqref="Z4"/>
+    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
+      <selection activeCell="BZ4" sqref="BZ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4" outlineLevelRow="3"/>
@@ -1329,6 +2440,7 @@
     <col min="11" max="11" width="16.8333333333333" customWidth="1"/>
     <col min="12" max="12" width="9.88888888888889" customWidth="1"/>
     <col min="14" max="14" width="10.4444444444444" customWidth="1"/>
+    <col min="64" max="64" width="20.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1336,7 +2448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="12.65" customHeight="1" spans="2:53">
+    <row r="2" s="1" customFormat="1" ht="12.65" customHeight="1" spans="2:293">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1403,174 +2515,1182 @@
       <c r="AY2" s="3"/>
       <c r="AZ2" s="3"/>
       <c r="BA2" s="3"/>
+      <c r="BB2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="BC2" s="5"/>
+      <c r="BD2" s="5"/>
+      <c r="BE2" s="5"/>
+      <c r="BF2" s="5"/>
+      <c r="BG2" s="5"/>
+      <c r="BH2" s="5"/>
+      <c r="BI2" s="5"/>
+      <c r="BJ2" s="5"/>
+      <c r="BK2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BL2" s="5"/>
+      <c r="BM2" s="5"/>
+      <c r="BN2" s="5"/>
+      <c r="BO2" s="5"/>
+      <c r="BP2" s="5"/>
+      <c r="BQ2" s="5"/>
+      <c r="BR2" s="5"/>
+      <c r="BS2" s="5"/>
+      <c r="BT2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="BU2" s="5"/>
+      <c r="BV2" s="5"/>
+      <c r="BW2" s="5"/>
+      <c r="BX2" s="5"/>
+      <c r="BY2" s="5"/>
+      <c r="BZ2" s="5"/>
+      <c r="CA2" s="5"/>
+      <c r="CB2" s="5"/>
+      <c r="CC2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="CD2" s="5"/>
+      <c r="CE2" s="5"/>
+      <c r="CF2" s="5"/>
+      <c r="CG2" s="5"/>
+      <c r="CH2" s="5"/>
+      <c r="CI2" s="5"/>
+      <c r="CJ2" s="5"/>
+      <c r="CK2" s="5"/>
+      <c r="CL2" s="5"/>
+      <c r="CM2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="CN2" s="5"/>
+      <c r="CO2" s="5"/>
+      <c r="CP2" s="5"/>
+      <c r="CQ2" s="5"/>
+      <c r="CR2" s="5"/>
+      <c r="CS2" s="5"/>
+      <c r="CT2" s="5"/>
+      <c r="CU2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="CV2" s="5"/>
+      <c r="CW2" s="5"/>
+      <c r="CX2" s="5"/>
+      <c r="CY2" s="5"/>
+      <c r="CZ2" s="5"/>
+      <c r="DA2" s="5"/>
+      <c r="DB2" s="5"/>
+      <c r="DC2" s="5"/>
+      <c r="DD2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="DE2" s="5"/>
+      <c r="DF2" s="5"/>
+      <c r="DG2" s="5"/>
+      <c r="DH2" s="5"/>
+      <c r="DI2" s="5"/>
+      <c r="DJ2" s="5"/>
+      <c r="DK2" s="5"/>
+      <c r="DL2" s="5"/>
+      <c r="DM2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="DN2" s="5"/>
+      <c r="DO2" s="5"/>
+      <c r="DP2" s="5"/>
+      <c r="DQ2" s="5"/>
+      <c r="DR2" s="5"/>
+      <c r="DS2" s="5"/>
+      <c r="DT2" s="5"/>
+      <c r="DU2" s="5"/>
+      <c r="DV2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="DW2" s="5"/>
+      <c r="DX2" s="5"/>
+      <c r="DY2" s="5"/>
+      <c r="DZ2" s="5"/>
+      <c r="EA2" s="5"/>
+      <c r="EB2" s="5"/>
+      <c r="EC2" s="5"/>
+      <c r="ED2" s="5"/>
+      <c r="EE2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="EF2" s="5"/>
+      <c r="EG2" s="5"/>
+      <c r="EH2" s="5"/>
+      <c r="EI2" s="5"/>
+      <c r="EJ2" s="5"/>
+      <c r="EK2" s="5"/>
+      <c r="EL2" s="5"/>
+      <c r="EM2" s="5"/>
+      <c r="EN2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="EO2" s="5"/>
+      <c r="EP2" s="5"/>
+      <c r="EQ2" s="5"/>
+      <c r="ER2" s="5"/>
+      <c r="ES2" s="5"/>
+      <c r="ET2" s="5"/>
+      <c r="EU2" s="5"/>
+      <c r="EV2" s="5"/>
+      <c r="EW2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="EX2" s="5"/>
+      <c r="EY2" s="5"/>
+      <c r="EZ2" s="5"/>
+      <c r="FA2" s="5"/>
+      <c r="FB2" s="5"/>
+      <c r="FC2" s="5"/>
+      <c r="FD2" s="5"/>
+      <c r="FE2" s="5"/>
+      <c r="FF2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="FG2" s="5"/>
+      <c r="FH2" s="5"/>
+      <c r="FI2" s="5"/>
+      <c r="FJ2" s="5"/>
+      <c r="FK2" s="5"/>
+      <c r="FL2" s="5"/>
+      <c r="FM2" s="5"/>
+      <c r="FN2" s="5"/>
+      <c r="FO2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="FP2" s="5"/>
+      <c r="FQ2" s="5"/>
+      <c r="FR2" s="5"/>
+      <c r="FS2" s="5"/>
+      <c r="FT2" s="5"/>
+      <c r="FU2" s="5"/>
+      <c r="FV2" s="5"/>
+      <c r="FW2" s="5"/>
+      <c r="FX2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="FY2" s="5"/>
+      <c r="FZ2" s="5"/>
+      <c r="GA2" s="5"/>
+      <c r="GB2" s="5"/>
+      <c r="GC2" s="5"/>
+      <c r="GD2" s="5"/>
+      <c r="GE2" s="5"/>
+      <c r="GF2" s="5"/>
+      <c r="GG2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="GH2" s="5"/>
+      <c r="GI2" s="5"/>
+      <c r="GJ2" s="5"/>
+      <c r="GK2" s="5"/>
+      <c r="GL2" s="5"/>
+      <c r="GM2" s="5"/>
+      <c r="GN2" s="5"/>
+      <c r="GO2" s="5"/>
+      <c r="GP2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="GQ2" s="5"/>
+      <c r="GR2" s="5"/>
+      <c r="GS2" s="5"/>
+      <c r="GT2" s="5"/>
+      <c r="GU2" s="5"/>
+      <c r="GV2" s="5"/>
+      <c r="GW2" s="5"/>
+      <c r="GX2" s="5"/>
+      <c r="GY2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="GZ2" s="5"/>
+      <c r="HA2" s="5"/>
+      <c r="HB2" s="5"/>
+      <c r="HC2" s="5"/>
+      <c r="HD2" s="5"/>
+      <c r="HE2" s="5"/>
+      <c r="HF2" s="5"/>
+      <c r="HG2" s="5"/>
+      <c r="HH2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="HI2" s="5"/>
+      <c r="HJ2" s="5"/>
+      <c r="HK2" s="5"/>
+      <c r="HL2" s="5"/>
+      <c r="HM2" s="5"/>
+      <c r="HN2" s="5"/>
+      <c r="HO2" s="5"/>
+      <c r="HP2" s="5"/>
+      <c r="HQ2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="HR2" s="5"/>
+      <c r="HS2" s="5"/>
+      <c r="HT2" s="5"/>
+      <c r="HU2" s="5"/>
+      <c r="HV2" s="5"/>
+      <c r="HW2" s="5"/>
+      <c r="HX2" s="5"/>
+      <c r="HY2" s="5"/>
+      <c r="HZ2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="IA2" s="5"/>
+      <c r="IB2" s="5"/>
+      <c r="IC2" s="5"/>
+      <c r="ID2" s="5"/>
+      <c r="IE2" s="5"/>
+      <c r="IF2" s="5"/>
+      <c r="IG2" s="5"/>
+      <c r="IH2" s="5"/>
+      <c r="II2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="IJ2" s="5"/>
+      <c r="IK2" s="5"/>
+      <c r="IL2" s="5"/>
+      <c r="IM2" s="5"/>
+      <c r="IN2" s="5"/>
+      <c r="IO2" s="5"/>
+      <c r="IP2" s="5"/>
+      <c r="IQ2" s="5"/>
+      <c r="IR2" s="5"/>
+      <c r="IS2" s="5"/>
+      <c r="IT2" s="5"/>
+      <c r="IU2" s="5"/>
+      <c r="IV2" s="5"/>
+      <c r="IW2" s="5"/>
+      <c r="IX2" s="5"/>
+      <c r="IY2" s="5"/>
+      <c r="IZ2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="JA2" s="5"/>
+      <c r="JB2" s="5"/>
+      <c r="JC2" s="5"/>
+      <c r="JD2" s="5"/>
+      <c r="JE2" s="5"/>
+      <c r="JF2" s="5"/>
+      <c r="JG2" s="5"/>
+      <c r="JH2" s="5"/>
+      <c r="JI2" s="5"/>
+      <c r="JJ2" s="5"/>
+      <c r="JK2" s="5"/>
+      <c r="JL2" s="5"/>
+      <c r="JM2" s="5"/>
+      <c r="JN2" s="5"/>
+      <c r="JO2" s="5"/>
+      <c r="JP2" s="5"/>
+      <c r="JQ2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="JR2" s="5"/>
+      <c r="JS2" s="5"/>
+      <c r="JT2" s="5"/>
+      <c r="JU2" s="5"/>
+      <c r="JV2" s="5"/>
+      <c r="JW2" s="5"/>
+      <c r="JX2" s="5"/>
+      <c r="JY2" s="5"/>
+      <c r="JZ2" s="5"/>
+      <c r="KA2" s="5"/>
+      <c r="KB2" s="5"/>
+      <c r="KC2" s="5"/>
+      <c r="KD2" s="5"/>
+      <c r="KE2" s="5"/>
+      <c r="KF2" s="5"/>
+      <c r="KG2" s="5"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="43.2" spans="1:53">
+    <row r="3" s="1" customFormat="1" ht="57.6" spans="1:293">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="AQ3" s="1" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="AS3" s="1" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="AW3" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="AZ3" s="1" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="BA3" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BH3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BI3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BO3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BP3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BQ3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BR3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BS3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="BU3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BV3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BX3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="BY3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BZ3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CA3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CB3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CC3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="CE3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CI3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CJ3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CK3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="CM3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="CN3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="CO3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CP3" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CQ3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="CR3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CS3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CT3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CU3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="CV3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="CW3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="CX3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="CY3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="CZ3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DA3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="DB3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="DC3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="DD3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="DE3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DF3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="DG3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DH3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DI3" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DJ3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="DK3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="DL3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="DM3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DN3" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="DO3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="DP3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DQ3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DR3" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DS3" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="DT3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="DU3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="DV3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DW3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="DX3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="DY3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="DZ3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="EA3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="EB3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="EC3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="ED3" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EE3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EF3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EG3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="EH3" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="EI3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="EJ3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="EK3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="EL3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="EM3" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="EN3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="EO3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="EP3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="EQ3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="ER3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="ES3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="ET3" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="EU3" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="EV3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="EW3" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="EX3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="EY3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="EZ3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="FA3" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="FB3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="FC3" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="FD3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="FE3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="FF3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="FG3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="FH3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="FI3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="FJ3" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="FK3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="FL3" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="FM3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="FN3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="FO3" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="FP3" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="FQ3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="FR3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="FS3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="FT3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="FU3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="FV3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="FW3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="FX3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="FY3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="FZ3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="GA3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="GB3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="GC3" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="GD3" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="GE3" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="GF3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="GG3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="GH3" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="GI3" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="GJ3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="GK3" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="GL3" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="GM3" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="GN3" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="GO3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="GP3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="GQ3" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="GR3" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="GS3" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="GT3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="GU3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="GV3" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="GW3" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="GX3" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="GY3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="GZ3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="HA3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="HB3" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="HC3" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="HD3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="HE3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="HF3" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="HG3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="HH3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="HI3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="HJ3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="HK3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="HL3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="HM3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="HN3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="HO3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="HP3" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="HQ3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="HR3" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="HS3" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="HT3" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="HU3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="HV3" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="HW3" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="HX3" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="HY3" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="HZ3" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="IA3" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="IB3" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="IC3" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="ID3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="IE3" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="IF3" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="IG3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="IH3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="II3" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="IJ3" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="IK3" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="IL3" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="IM3" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="IN3" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="IO3" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="IP3" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="IQ3" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="IR3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="IS3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="IT3" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="IU3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="IV3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="IW3" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="IX3" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="IY3" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="IZ3" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="JA3" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="JB3" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="JC3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="JD3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="JE3" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="JF3" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="JG3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="JH3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="JI3" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="JJ3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="JK3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="JL3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="JM3" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="JN3" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="JO3" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="JP3" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="JQ3" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="JR3" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="JS3" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="JT3" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="JU3" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="JV3" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="JW3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="JX3" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="JY3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="JZ3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="KA3" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="KB3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="KC3" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="KD3" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="KE3" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="KF3" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="KG3" s="1" t="s">
+        <v>324</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" ht="230.4" spans="1:53">
+    <row r="4" s="2" customFormat="1" ht="287" customHeight="1" spans="1:293">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>325</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>326</v>
       </c>
       <c r="C4" s="2">
         <v>1561290</v>
@@ -1579,16 +3699,16 @@
         <v>20880</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>327</v>
       </c>
       <c r="F4">
         <v>5829372829</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>328</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>65</v>
+        <v>329</v>
       </c>
       <c r="I4" s="4">
         <v>45650.7493171296</v>
@@ -1597,7 +3717,7 @@
         <v>89</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>66</v>
+        <v>330</v>
       </c>
       <c r="L4" s="2">
         <v>1</v>
@@ -1725,9 +3845,729 @@
       <c r="BA4" s="2">
         <v>33.333</v>
       </c>
+      <c r="BB4" s="2">
+        <v>146440</v>
+      </c>
+      <c r="BC4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="BD4" s="2">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="BG4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="BH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="BI4" s="2">
+        <v>1</v>
+      </c>
+      <c r="BJ4" s="2">
+        <v>1</v>
+      </c>
+      <c r="BK4" s="2">
+        <v>136095</v>
+      </c>
+      <c r="BL4" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="BM4" s="2">
+        <v>4</v>
+      </c>
+      <c r="BN4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="BO4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="BP4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="BQ4" s="2">
+        <v>0</v>
+      </c>
+      <c r="BR4" s="2">
+        <v>1</v>
+      </c>
+      <c r="BS4" s="2">
+        <v>1</v>
+      </c>
+      <c r="BT4" s="2">
+        <v>136097</v>
+      </c>
+      <c r="BU4" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="BV4" s="2">
+        <v>3</v>
+      </c>
+      <c r="BW4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="BX4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="BY4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="BZ4" s="2">
+        <v>0</v>
+      </c>
+      <c r="CA4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CC4" s="2">
+        <v>146436</v>
+      </c>
+      <c r="CD4" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="CE4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CF4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="CG4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="CH4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="CI4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CJ4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CK4" s="2">
+        <v>2</v>
+      </c>
+      <c r="CL4" s="2">
+        <v>146438</v>
+      </c>
+      <c r="CM4" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="CN4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CO4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="CP4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="CQ4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="CR4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CS4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CT4" s="2">
+        <v>1</v>
+      </c>
+      <c r="CU4" s="2">
+        <v>141429</v>
+      </c>
+      <c r="CV4" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="CW4" s="2">
+        <v>4</v>
+      </c>
+      <c r="CX4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="CY4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="CZ4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="DA4" s="2">
+        <v>0</v>
+      </c>
+      <c r="DB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="DC4" s="2">
+        <v>1</v>
+      </c>
+      <c r="DD4" s="2">
+        <v>141431</v>
+      </c>
+      <c r="DE4" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="DF4" s="2">
+        <v>4</v>
+      </c>
+      <c r="DG4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="DH4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="DI4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="DJ4" s="2">
+        <v>0</v>
+      </c>
+      <c r="DK4" s="2">
+        <v>1</v>
+      </c>
+      <c r="DL4" s="2">
+        <v>1</v>
+      </c>
+      <c r="DM4" s="2">
+        <v>141419</v>
+      </c>
+      <c r="DN4" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="DO4" s="2">
+        <v>3</v>
+      </c>
+      <c r="DP4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="DQ4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="DR4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="DS4" s="2">
+        <v>0</v>
+      </c>
+      <c r="DT4" s="2">
+        <v>1</v>
+      </c>
+      <c r="DU4" s="2">
+        <v>1</v>
+      </c>
+      <c r="DV4" s="2">
+        <v>141421</v>
+      </c>
+      <c r="DW4" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="DX4" s="2">
+        <v>3</v>
+      </c>
+      <c r="DY4" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="DZ4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="EA4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="EB4" s="2">
+        <v>0</v>
+      </c>
+      <c r="EC4" s="2">
+        <v>1</v>
+      </c>
+      <c r="ED4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EE4" s="2">
+        <v>146450</v>
+      </c>
+      <c r="EF4" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="EG4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EH4" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="EI4" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="EJ4" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="EK4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EL4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EM4" s="2">
+        <v>19</v>
+      </c>
+      <c r="EN4" s="2">
+        <v>141573</v>
+      </c>
+      <c r="EO4" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="EP4" s="2">
+        <v>4</v>
+      </c>
+      <c r="EQ4" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="ER4" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="ES4" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="ET4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EU4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EV4" s="2">
+        <v>21</v>
+      </c>
+      <c r="EW4" s="2">
+        <v>141575</v>
+      </c>
+      <c r="EX4" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="EY4" s="2">
+        <v>3</v>
+      </c>
+      <c r="EZ4" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="FA4" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="FB4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="FC4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FD4" s="2">
+        <v>1</v>
+      </c>
+      <c r="FE4" s="2">
+        <v>21</v>
+      </c>
+      <c r="FF4" s="2">
+        <v>146442</v>
+      </c>
+      <c r="FG4" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="FH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="FI4" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="FJ4" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="FK4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="FL4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FM4" s="2">
+        <v>1</v>
+      </c>
+      <c r="FN4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FO4" s="2">
+        <v>141667</v>
+      </c>
+      <c r="FP4" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="FQ4" s="2">
+        <v>4</v>
+      </c>
+      <c r="FR4" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="FS4" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="FT4" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="FU4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FV4" s="2">
+        <v>1</v>
+      </c>
+      <c r="FW4" s="2">
+        <v>0</v>
+      </c>
+      <c r="FX4" s="2">
+        <v>141693</v>
+      </c>
+      <c r="FY4" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="FZ4" s="2">
+        <v>3</v>
+      </c>
+      <c r="GA4" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="GB4" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="GC4" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="GD4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GE4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GF4" s="2">
+        <v>0</v>
+      </c>
+      <c r="GG4" s="2">
+        <v>146444</v>
+      </c>
+      <c r="GH4" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="GI4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GJ4" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="GK4" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="GL4" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="GM4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GN4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GO4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GP4" s="2">
+        <v>142459</v>
+      </c>
+      <c r="GQ4" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="GR4" s="2">
+        <v>4</v>
+      </c>
+      <c r="GS4" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="GT4" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="GU4" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="GV4" s="2">
+        <v>0</v>
+      </c>
+      <c r="GW4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GX4" s="2">
+        <v>0</v>
+      </c>
+      <c r="GY4" s="2">
+        <v>142463</v>
+      </c>
+      <c r="GZ4" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="HA4" s="2">
+        <v>3</v>
+      </c>
+      <c r="HB4" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="HC4" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="HD4" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="HE4" s="2">
+        <v>0</v>
+      </c>
+      <c r="HF4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HG4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HH4" s="2">
+        <v>146446</v>
+      </c>
+      <c r="HI4" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="HJ4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HK4" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="HL4" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="HM4" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="HN4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HO4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HP4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HQ4" s="2">
+        <v>142461</v>
+      </c>
+      <c r="HR4" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="HS4" s="2">
+        <v>4</v>
+      </c>
+      <c r="HT4" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="HU4" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="HV4" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="HW4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="HX4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HY4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HZ4" s="2">
+        <v>142465</v>
+      </c>
+      <c r="IA4" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="IB4" s="2">
+        <v>3</v>
+      </c>
+      <c r="IC4" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="ID4" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="IE4" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="IF4" s="2">
+        <v>0</v>
+      </c>
+      <c r="IG4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="II4" s="2">
+        <v>146448</v>
+      </c>
+      <c r="IJ4" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="IK4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IL4" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="IM4" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="IN4" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="IO4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IP4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IQ4" s="2">
+        <v>6</v>
+      </c>
+      <c r="IR4" s="2">
+        <v>8</v>
+      </c>
+      <c r="IS4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IT4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IU4" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="IV4" s="2">
+        <v>0.0027</v>
+      </c>
+      <c r="IW4" s="2">
+        <v>1920</v>
+      </c>
+      <c r="IX4" s="2">
+        <v>4</v>
+      </c>
+      <c r="IY4" s="2">
+        <v>0</v>
+      </c>
+      <c r="IZ4" s="2">
+        <v>142593</v>
+      </c>
+      <c r="JA4" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="JB4" s="2">
+        <v>4</v>
+      </c>
+      <c r="JC4" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="JD4" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="JE4" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="JF4" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="JG4" s="2">
+        <v>1</v>
+      </c>
+      <c r="JH4" s="2">
+        <v>6</v>
+      </c>
+      <c r="JI4" s="2">
+        <v>12</v>
+      </c>
+      <c r="JJ4" s="2">
+        <v>2</v>
+      </c>
+      <c r="JK4" s="2">
+        <v>1</v>
+      </c>
+      <c r="JL4" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="JM4" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="JN4" s="2">
+        <v>25024</v>
+      </c>
+      <c r="JO4" s="2">
+        <v>1</v>
+      </c>
+      <c r="JP4" s="2">
+        <v>1</v>
+      </c>
+      <c r="JQ4" s="2">
+        <v>142591</v>
+      </c>
+      <c r="JR4" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="JS4" s="2">
+        <v>3</v>
+      </c>
+      <c r="JT4" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="JU4" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="JV4" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="JW4" s="2">
+        <v>0</v>
+      </c>
+      <c r="JX4" s="2">
+        <v>1</v>
+      </c>
+      <c r="JY4" s="2">
+        <v>1</v>
+      </c>
+      <c r="JZ4" s="2">
+        <v>12</v>
+      </c>
+      <c r="KA4" s="2">
+        <v>2</v>
+      </c>
+      <c r="KB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="KC4" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="KD4" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="KE4" s="2">
+        <v>25024</v>
+      </c>
+      <c r="KF4" s="2">
+        <v>1</v>
+      </c>
+      <c r="KG4" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="31">
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="I2:R2"/>
     <mergeCell ref="S2:Y2"/>
@@ -1735,6 +4575,30 @@
     <mergeCell ref="AG2:AM2"/>
     <mergeCell ref="AN2:AT2"/>
     <mergeCell ref="AU2:BA2"/>
+    <mergeCell ref="BB2:BJ2"/>
+    <mergeCell ref="BK2:BS2"/>
+    <mergeCell ref="BT2:CB2"/>
+    <mergeCell ref="CC2:CL2"/>
+    <mergeCell ref="CM2:CT2"/>
+    <mergeCell ref="CU2:DC2"/>
+    <mergeCell ref="DD2:DL2"/>
+    <mergeCell ref="DM2:DU2"/>
+    <mergeCell ref="DV2:ED2"/>
+    <mergeCell ref="EE2:EM2"/>
+    <mergeCell ref="EN2:EV2"/>
+    <mergeCell ref="EW2:FE2"/>
+    <mergeCell ref="FF2:FN2"/>
+    <mergeCell ref="FO2:FW2"/>
+    <mergeCell ref="FX2:GF2"/>
+    <mergeCell ref="GG2:GO2"/>
+    <mergeCell ref="GP2:GX2"/>
+    <mergeCell ref="GY2:HG2"/>
+    <mergeCell ref="HH2:HP2"/>
+    <mergeCell ref="HQ2:HY2"/>
+    <mergeCell ref="HZ2:IH2"/>
+    <mergeCell ref="II2:IY2"/>
+    <mergeCell ref="IZ2:JP2"/>
+    <mergeCell ref="JQ2:KG2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" display="https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png" tooltip="https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png"/>

</xml_diff>

<commit_message>
write excel issue fix
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
@@ -1045,7 +1045,7 @@
 </t>
   </si>
   <si>
-    <t>Skipped</t>
+    <t>EMPTY</t>
   </si>
   <si>
     <t>child q1 sa automation /ans : A</t>
@@ -1323,19 +1323,12 @@
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1812,142 +1805,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1971,7 +1964,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2426,7 +2418,7 @@
   <dimension ref="A1:KG4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BZ4" sqref="BZ4"/>
+      <selection activeCell="BX4" sqref="BX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4" outlineLevelRow="3"/>
@@ -4103,7 +4095,7 @@
       <c r="EI4" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="EJ4" s="8" t="s">
+      <c r="EJ4" s="6" t="s">
         <v>349</v>
       </c>
       <c r="EK4" s="2">
@@ -4130,7 +4122,7 @@
       <c r="ER4" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="ES4" s="8" t="s">
+      <c r="ES4" s="6" t="s">
         <v>351</v>
       </c>
       <c r="ET4" s="2">
@@ -4235,7 +4227,7 @@
       <c r="GA4" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="GB4" s="9" t="s">
+      <c r="GB4" s="8" t="s">
         <v>361</v>
       </c>
       <c r="GC4" s="2" t="s">
@@ -4475,7 +4467,7 @@
       <c r="JC4" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="JD4" s="8" t="s">
+      <c r="JD4" s="6" t="s">
         <v>384</v>
       </c>
       <c r="JE4" s="2" t="s">
@@ -4526,7 +4518,7 @@
       <c r="JT4" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="JU4" s="8" t="s">
+      <c r="JU4" s="6" t="s">
         <v>387</v>
       </c>
       <c r="JV4" s="2" t="s">

</xml_diff>

<commit_message>
selfassessment webreport final + miccheck more cases added
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="388">
   <si>
     <t>Candidate Transcript Report</t>
   </si>
@@ -1013,7 +1013,7 @@
     <t>qatesthirepro@gmail.com</t>
   </si>
   <si>
-    <t>None</t>
+    <t>EMPTY</t>
   </si>
   <si>
     <t>https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png</t>
@@ -1043,9 +1043,6 @@
   <si>
     <t xml:space="preserve">don't use po mcq automation hirepro question self assessment
 </t>
-  </si>
-  <si>
-    <t>EMPTY</t>
   </si>
   <si>
     <t>child q1 sa automation /ans : A</t>
@@ -2417,8 +2414,8 @@
   <sheetPr/>
   <dimension ref="A1:KG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BO1" workbookViewId="0">
-      <selection activeCell="BX4" sqref="BX4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4" outlineLevelRow="3"/>
@@ -3907,7 +3904,7 @@
         <v>336</v>
       </c>
       <c r="BY4" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="BZ4" s="2">
         <v>0</v>
@@ -3922,7 +3919,7 @@
         <v>146436</v>
       </c>
       <c r="CD4" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="CE4" s="2">
         <v>1</v>
@@ -3949,7 +3946,7 @@
         <v>146438</v>
       </c>
       <c r="CM4" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="CN4" s="2">
         <v>1</v>
@@ -3976,7 +3973,7 @@
         <v>141429</v>
       </c>
       <c r="CV4" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="CW4" s="2">
         <v>4</v>
@@ -4003,7 +4000,7 @@
         <v>141431</v>
       </c>
       <c r="DE4" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="DF4" s="2">
         <v>4</v>
@@ -4015,7 +4012,7 @@
         <v>333</v>
       </c>
       <c r="DI4" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="DJ4" s="2">
         <v>0</v>
@@ -4030,7 +4027,7 @@
         <v>141419</v>
       </c>
       <c r="DN4" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="DO4" s="2">
         <v>3</v>
@@ -4042,7 +4039,7 @@
         <v>336</v>
       </c>
       <c r="DR4" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="DS4" s="2">
         <v>0</v>
@@ -4057,7 +4054,7 @@
         <v>141421</v>
       </c>
       <c r="DW4" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="DX4" s="2">
         <v>3</v>
@@ -4069,7 +4066,7 @@
         <v>335</v>
       </c>
       <c r="EA4" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="EB4" s="2">
         <v>0</v>
@@ -4084,19 +4081,19 @@
         <v>146450</v>
       </c>
       <c r="EF4" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="EG4" s="2">
+        <v>1</v>
+      </c>
+      <c r="EH4" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="EG4" s="2">
-        <v>1</v>
-      </c>
-      <c r="EH4" s="2" t="s">
+      <c r="EI4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="EI4" s="2" t="s">
+      <c r="EJ4" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="EJ4" s="6" t="s">
-        <v>349</v>
       </c>
       <c r="EK4" s="2">
         <v>1</v>
@@ -4111,19 +4108,19 @@
         <v>141573</v>
       </c>
       <c r="EO4" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="EP4" s="2">
         <v>4</v>
       </c>
       <c r="EQ4" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="ER4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="ER4" s="2" t="s">
-        <v>348</v>
-      </c>
       <c r="ES4" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="ET4" s="2">
         <v>1</v>
@@ -4138,19 +4135,19 @@
         <v>141575</v>
       </c>
       <c r="EX4" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="EY4" s="2">
         <v>3</v>
       </c>
       <c r="EZ4" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="FA4" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="FB4" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="FC4" s="2">
         <v>0</v>
@@ -4165,19 +4162,19 @@
         <v>146442</v>
       </c>
       <c r="FG4" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="FH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="FI4" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="FH4" s="2">
-        <v>1</v>
-      </c>
-      <c r="FI4" s="2" t="s">
+      <c r="FJ4" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="FJ4" s="6" t="s">
-        <v>356</v>
-      </c>
       <c r="FK4" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="FL4" s="2">
         <v>0</v>
@@ -4192,19 +4189,19 @@
         <v>141667</v>
       </c>
       <c r="FP4" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="FQ4" s="2">
         <v>4</v>
       </c>
       <c r="FR4" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="FS4" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="FT4" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="FT4" s="2" t="s">
-        <v>359</v>
       </c>
       <c r="FU4" s="2">
         <v>0</v>
@@ -4219,19 +4216,19 @@
         <v>141693</v>
       </c>
       <c r="FY4" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="FZ4" s="2">
         <v>3</v>
       </c>
       <c r="GA4" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="GB4" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="GC4" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="GC4" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="GD4" s="2">
         <v>1</v>
@@ -4246,19 +4243,19 @@
         <v>146444</v>
       </c>
       <c r="GH4" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="GI4" s="2">
+        <v>1</v>
+      </c>
+      <c r="GJ4" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="GI4" s="2">
-        <v>1</v>
-      </c>
-      <c r="GJ4" s="2" t="s">
+      <c r="GK4" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="GK4" s="2" t="s">
+      <c r="GL4" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="GL4" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="GM4" s="2">
         <v>1</v>
@@ -4273,19 +4270,19 @@
         <v>142459</v>
       </c>
       <c r="GQ4" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="GR4" s="2">
         <v>4</v>
       </c>
       <c r="GS4" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="GT4" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="GU4" s="2" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="GV4" s="2">
         <v>0</v>
@@ -4300,19 +4297,19 @@
         <v>142463</v>
       </c>
       <c r="GZ4" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="HA4" s="2">
         <v>3</v>
       </c>
       <c r="HB4" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="HC4" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="HD4" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="HD4" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="HE4" s="2">
         <v>0</v>
@@ -4327,16 +4324,16 @@
         <v>146446</v>
       </c>
       <c r="HI4" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="HJ4" s="2">
+        <v>1</v>
+      </c>
+      <c r="HK4" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="HJ4" s="2">
-        <v>1</v>
-      </c>
-      <c r="HK4" s="2" t="s">
+      <c r="HL4" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="HL4" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="HM4" s="2" t="s">
         <v>333</v>
@@ -4354,16 +4351,16 @@
         <v>142461</v>
       </c>
       <c r="HR4" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="HS4" s="2">
         <v>4</v>
       </c>
       <c r="HT4" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="HU4" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="HU4" s="2" t="s">
-        <v>374</v>
       </c>
       <c r="HV4" s="2" t="s">
         <v>336</v>
@@ -4381,19 +4378,19 @@
         <v>142465</v>
       </c>
       <c r="IA4" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="IB4" s="2">
         <v>3</v>
       </c>
       <c r="IC4" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="ID4" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="IE4" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="IF4" s="2">
         <v>0</v>
@@ -4408,19 +4405,19 @@
         <v>146448</v>
       </c>
       <c r="IJ4" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="IK4" s="2">
+        <v>1</v>
+      </c>
+      <c r="IL4" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="IK4" s="2">
-        <v>1</v>
-      </c>
-      <c r="IL4" s="2" t="s">
+      <c r="IM4" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="IM4" s="2" t="s">
+      <c r="IN4" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="IN4" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="IO4" s="2">
         <v>1</v>
@@ -4441,7 +4438,7 @@
         <v>1</v>
       </c>
       <c r="IU4" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="IV4" s="2">
         <v>0.0027</v>
@@ -4459,19 +4456,19 @@
         <v>142593</v>
       </c>
       <c r="JA4" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="JB4" s="2">
         <v>4</v>
       </c>
       <c r="JC4" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="JD4" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="JE4" s="2" t="s">
         <v>384</v>
-      </c>
-      <c r="JE4" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="JF4" s="2">
         <v>0.5</v>
@@ -4492,7 +4489,7 @@
         <v>1</v>
       </c>
       <c r="JL4" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="JM4" s="2">
         <v>0.06</v>
@@ -4510,19 +4507,19 @@
         <v>142591</v>
       </c>
       <c r="JR4" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="JS4" s="2">
         <v>3</v>
       </c>
       <c r="JT4" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="JU4" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="JV4" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="JV4" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="JW4" s="2">
         <v>0</v>
@@ -4543,7 +4540,7 @@
         <v>1</v>
       </c>
       <c r="KC4" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="KD4" s="2">
         <v>0.06</v>

</xml_diff>

<commit_message>
assessment and authoring grid actions
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
+++ b/PythonWorkingScripts_InputData/Assessment/selfassessment_report/selfassessment_generic_webreport.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9120" tabRatio="500"/>
+    <workbookView windowWidth="19890" windowHeight="7620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1016,7 +1016,7 @@
     <t>EMPTY</t>
   </si>
   <si>
-    <t>https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png</t>
+    <t>https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png</t>
   </si>
   <si>
     <t>103.215.237.219</t>
@@ -1082,10 +1082,10 @@
     <t>{
   "textArea1": "I am very foodie. I love to eat. Among the number of foods, Pizza is my favourite food because it tastes and smells fabulous. My Mom cooks the best Pizzas in the world. I always ask her to make Pizza. In Pizzas, I love onion cheese Pizza a lot. This is because cheese pizza is healthy and makes me strong. To create fun we also organize pizza races in terms of who can eat the maximum number of pizzas. I can eat many pizzas at a time.",
   "capture1": [
-    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/d61a25e6-defa-4618-886d-9633fa6c9584photoCapture0.png"
+    "https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/d61a25e6-defa-4618-886d-9633fa6c9584photoCapture0.png"
   ],
   "attachment1": [
-    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/f783bacc-d9d1-43e0-9e41-508cf06a50b6self_assessment.xls"
+    "https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/f783bacc-d9d1-43e0-9e41-508cf06a50b6self_assessment.xls"
   ]
 }</t>
   </si>
@@ -1098,10 +1098,10 @@
     <t>{
   "textArea1": "I am very foodie. I love to eat. Among the number of foods, Pizza is my favourite food because it tastes and smells fabulous. My Mom cooks the best Pizzas in the world. I always ask her to make Pizza. In Pizzas, I love onion cheese Pizza a lot. This is because cheese pizza is healthy and makes me strong. To create fun we also organize pizza races in terms of who can eat the maximum number of pizzas. I can eat many pizzas at a time.",
   "capture1": [
-    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/3efd239a-947f-43a4-a42a-ddcf47ec0e5aphotoCapture0.png"
+    "https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/3efd239a-947f-43a4-a42a-ddcf47ec0e5aphotoCapture0.png"
   ],
   "attachment1": [
-    "https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/6eee099d-232a-45a8-8f4e-da46f8441c46self_assessment.xls"
+    "https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/testResultAnswers/20880/1561290/6eee099d-232a-45a8-8f4e-da46f8441c46self_assessment.xls"
   ]
 }</t>
   </si>
@@ -1314,11 +1314,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\Thh:mm:ss"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="yyyy/mm/dd\Thh:mm:ss"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1802,11 +1802,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1950,7 +1950,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2414,22 +2414,22 @@
   <sheetPr/>
   <dimension ref="A1:KG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="EG3" workbookViewId="0">
+      <selection activeCell="EQ4" sqref="EQ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89814814814815" defaultRowHeight="14.4" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="8.8952380952381" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="2" max="2" width="24.8981481481481" customWidth="1"/>
-    <col min="6" max="6" width="14.6018518518519" customWidth="1"/>
-    <col min="7" max="7" width="17.3888888888889" customWidth="1"/>
-    <col min="8" max="8" width="10.9907407407407" customWidth="1"/>
-    <col min="9" max="9" width="18.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="24.8952380952381" customWidth="1"/>
+    <col min="6" max="6" width="14.6" customWidth="1"/>
+    <col min="7" max="7" width="17.3904761904762" customWidth="1"/>
+    <col min="8" max="8" width="10.9904761904762" customWidth="1"/>
+    <col min="9" max="9" width="18.7809523809524" customWidth="1"/>
     <col min="10" max="10" width="14.3333333333333" customWidth="1"/>
-    <col min="11" max="11" width="16.8333333333333" customWidth="1"/>
-    <col min="12" max="12" width="9.88888888888889" customWidth="1"/>
-    <col min="14" max="14" width="10.4444444444444" customWidth="1"/>
-    <col min="64" max="64" width="20.8888888888889" customWidth="1"/>
+    <col min="11" max="11" width="16.8380952380952" customWidth="1"/>
+    <col min="12" max="12" width="9.88571428571429" customWidth="1"/>
+    <col min="14" max="14" width="10.447619047619" customWidth="1"/>
+    <col min="64" max="64" width="20.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2793,7 +2793,7 @@
       <c r="KF2" s="5"/>
       <c r="KG2" s="5"/>
     </row>
-    <row r="3" s="1" customFormat="1" ht="57.6" spans="1:293">
+    <row r="3" s="1" customFormat="1" ht="60" spans="1:293">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -4092,7 +4092,7 @@
       <c r="EI4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="EJ4" s="6" t="s">
+      <c r="EJ4" s="7" t="s">
         <v>348</v>
       </c>
       <c r="EK4" s="2">
@@ -4119,7 +4119,7 @@
       <c r="ER4" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="ES4" s="6" t="s">
+      <c r="ES4" s="7" t="s">
         <v>350</v>
       </c>
       <c r="ET4" s="2">
@@ -4590,7 +4590,7 @@
     <mergeCell ref="JQ2:KG2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" display="https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png" tooltip="https://s3-ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png"/>
+    <hyperlink ref="H4" r:id="rId1" display="https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png" tooltip="https://s3.ap-southeast-1.amazonaws.com/test-all-hirepro-files/crpodemo/Candidates/1561290/9373ee06-e557-451a-895d-67c07fa4fef1download__1_.png"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>